<commit_message>
Changed action code 'reverse' to 'cancel' to be more general in use.
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk/build@4778 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/source/processrequest/processrequest-spreadsheet.xlsx
+++ b/source/processrequest/processrequest-spreadsheet.xlsx
@@ -2561,7 +2561,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="213">
   <si>
     <t>FHIR Resource-authoring Spreadsheet</t>
   </si>
@@ -2767,9 +2767,6 @@
     <t>ProcessRequest.request</t>
   </si>
   <si>
-    <t>Reference(OralHealthClaim|PharmacyClaim|VisionClaim|ProfessionalClaim|InstitutionalClaim|SupportingDocumentation)</t>
-  </si>
-  <si>
     <t>Request reference</t>
   </si>
   <si>
@@ -2779,9 +2776,6 @@
     <t>ProcessRequest.response</t>
   </si>
   <si>
-    <t>Reference(ClaimResponse|StatusResponse)</t>
-  </si>
-  <si>
     <t>Response reference</t>
   </si>
   <si>
@@ -3203,6 +3197,9 @@
   </si>
   <si>
     <t>Required for Readjudicate</t>
+  </si>
+  <si>
+    <t>Reference(Any)</t>
   </si>
 </sst>
 </file>
@@ -4392,6 +4389,1035 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFA5A5A5"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA5A5A5"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA5A5A5"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA5A5A5"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA5A5A5"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA5A5A5"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA5A5A5"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA5A5A5"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFD8D8D8"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD8D8D8"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFD8D8D8"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFD8D8D8"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -4435,1035 +5461,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFA5A5A5"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA5A5A5"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA5A5A5"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA5A5A5"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA5A5A5"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA5A5A5"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA5A5A5"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA5A5A5"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA5A5A5"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFD8D8D8"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFD8D8D8"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFD8D8D8"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFD8D8D8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
       <border>
@@ -6401,7 +6398,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B1" s="46" t="s">
         <v>20</v>
@@ -6413,28 +6410,28 @@
         <v>15</v>
       </c>
       <c r="E1" s="46" t="s">
+        <v>199</v>
+      </c>
+      <c r="F1" s="46" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" s="46" t="s">
+        <v>200</v>
+      </c>
+      <c r="H1" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="F1" s="46" t="s">
-        <v>164</v>
-      </c>
-      <c r="G1" s="46" t="s">
+      <c r="I1" s="46" t="s">
         <v>202</v>
       </c>
-      <c r="H1" s="46" t="s">
+      <c r="J1" s="46" t="s">
         <v>203</v>
       </c>
-      <c r="I1" s="46" t="s">
+      <c r="K1" s="46" t="s">
         <v>204</v>
       </c>
-      <c r="J1" s="46" t="s">
+      <c r="L1" s="46" t="s">
         <v>205</v>
-      </c>
-      <c r="K1" s="46" t="s">
-        <v>206</v>
-      </c>
-      <c r="L1" s="46" t="s">
-        <v>207</v>
       </c>
       <c r="M1" s="47" t="s">
         <v>30</v>
@@ -6879,37 +6876,37 @@
   </sheetData>
   <autoFilter ref="A1:M1"/>
   <conditionalFormatting sqref="A2:M30">
-    <cfRule type="expression" dxfId="15" priority="0">
+    <cfRule type="expression" dxfId="12" priority="0">
       <formula>AND($A2="",A2&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A30">
-    <cfRule type="expression" dxfId="14" priority="0">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>AND(A2&lt;&gt;"",A1="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C30">
-    <cfRule type="expression" dxfId="13" priority="0">
+    <cfRule type="expression" dxfId="10" priority="2">
       <formula>AND($A2&lt;&gt;"",B2="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E30">
-    <cfRule type="expression" dxfId="12" priority="0">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>AND($A2&lt;&gt;"",($C2="unbound")&lt;&gt;(E2=""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F30">
-    <cfRule type="expression" dxfId="11" priority="0">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>AND($A2&lt;&gt;"",(F2&lt;&gt;"")&lt;&gt;($C2="reference"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:J30">
-    <cfRule type="expression" dxfId="10" priority="0">
+    <cfRule type="expression" dxfId="7" priority="5">
       <formula>AND(G2&lt;&gt;"",$C2&lt;&gt;"code list")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:M30">
-    <cfRule type="expression" dxfId="9" priority="0">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>LEFT($A2,1)="!"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6952,28 +6949,28 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
+        <v>206</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>207</v>
+      </c>
+      <c r="D1" s="46" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="46" t="s">
-        <v>155</v>
-      </c>
-      <c r="C1" s="46" t="s">
+      <c r="E1" s="46" t="s">
         <v>209</v>
-      </c>
-      <c r="D1" s="46" t="s">
-        <v>210</v>
-      </c>
-      <c r="E1" s="46" t="s">
-        <v>211</v>
       </c>
       <c r="F1" s="46" t="s">
         <v>20</v>
       </c>
       <c r="G1" s="46" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H1" s="46" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I1" s="47" t="s">
         <v>30</v>
@@ -7522,32 +7519,32 @@
   </sheetData>
   <autoFilter ref="A1:I1"/>
   <conditionalFormatting sqref="A2:I50">
-    <cfRule type="expression" dxfId="8" priority="0">
+    <cfRule type="expression" dxfId="5" priority="0">
       <formula>AND($A2="",A2&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A50">
-    <cfRule type="expression" dxfId="7" priority="0">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>AND(A2&lt;&gt;"",A1="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C50">
-    <cfRule type="expression" dxfId="6" priority="0">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>AND($A2&lt;&gt;"",($B2="")=($C2=""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:F50">
-    <cfRule type="expression" dxfId="5" priority="0">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>AND($A2&lt;&gt;"",$C2="",E2="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F50">
-    <cfRule type="expression" dxfId="4" priority="0">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>AND($A2&lt;&gt;"",,$C2="",$E2="",F2="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:I50">
-    <cfRule type="expression" dxfId="3" priority="0">
+    <cfRule type="expression" dxfId="0" priority="5">
       <formula>LEFT($A2,1)="!"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7561,10 +7558,10 @@
   <dimension ref="A1:AB101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H27" sqref="H27"/>
+      <selection pane="bottomRight" activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8042,7 +8039,7 @@
       <c r="AA10" s="29"/>
       <c r="AB10" s="31"/>
     </row>
-    <row r="11" spans="1:28" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
         <v>67</v>
       </c>
@@ -8056,7 +8053,7 @@
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26" t="s">
-        <v>68</v>
+        <v>212</v>
       </c>
       <c r="J11" s="26"/>
       <c r="K11" s="26"/>
@@ -8066,10 +8063,10 @@
       <c r="O11" s="26"/>
       <c r="P11" s="26"/>
       <c r="Q11" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="R11" s="27" t="s">
         <v>69</v>
-      </c>
-      <c r="R11" s="27" t="s">
-        <v>70</v>
       </c>
       <c r="S11" s="28"/>
       <c r="T11" s="27"/>
@@ -8084,7 +8081,7 @@
     </row>
     <row r="12" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="32"/>
       <c r="C12" s="32"/>
@@ -8096,7 +8093,7 @@
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26" t="s">
-        <v>72</v>
+        <v>212</v>
       </c>
       <c r="J12" s="26"/>
       <c r="K12" s="26"/>
@@ -8106,10 +8103,10 @@
       <c r="O12" s="26"/>
       <c r="P12" s="26"/>
       <c r="Q12" s="26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="R12" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S12" s="28"/>
       <c r="T12" s="27"/>
@@ -8124,7 +8121,7 @@
     </row>
     <row r="13" spans="1:28" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B13" s="25"/>
       <c r="C13" s="25"/>
@@ -8132,7 +8129,7 @@
       <c r="E13" s="25"/>
       <c r="F13" s="26"/>
       <c r="G13" s="26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H13" s="26"/>
       <c r="I13" s="26" t="s">
@@ -8146,10 +8143,10 @@
       <c r="O13" s="26"/>
       <c r="P13" s="26"/>
       <c r="Q13" s="26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="R13" s="27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S13" s="28"/>
       <c r="T13" s="27"/>
@@ -8164,7 +8161,7 @@
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="95" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B14" s="25"/>
       <c r="C14" s="25"/>
@@ -8196,7 +8193,7 @@
     </row>
     <row r="15" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="95" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B15" s="32"/>
       <c r="C15" s="25"/>
@@ -8208,7 +8205,7 @@
       </c>
       <c r="H15" s="26"/>
       <c r="I15" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J15" s="26"/>
       <c r="K15" s="26"/>
@@ -8218,10 +8215,10 @@
       <c r="O15" s="26"/>
       <c r="P15" s="26"/>
       <c r="Q15" s="26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="R15" s="27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="S15" s="28"/>
       <c r="T15" s="27"/>
@@ -8229,18 +8226,18 @@
       <c r="V15" s="29"/>
       <c r="W15" s="29"/>
       <c r="X15" s="29" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="Y15" s="29"/>
       <c r="Z15" s="30"/>
       <c r="AA15" s="29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AB15" s="31"/>
     </row>
     <row r="16" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="95" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B16" s="32"/>
       <c r="C16" s="25"/>
@@ -8257,17 +8254,17 @@
       <c r="J16" s="26"/>
       <c r="K16" s="26"/>
       <c r="L16" s="26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M16" s="26"/>
       <c r="N16" s="26"/>
       <c r="O16" s="26"/>
       <c r="P16" s="26"/>
       <c r="Q16" s="26" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="R16" s="27" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S16" s="28"/>
       <c r="T16" s="27"/>
@@ -8282,7 +8279,7 @@
     </row>
     <row r="17" spans="1:28" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="95" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B17" s="32"/>
       <c r="C17" s="25"/>
@@ -8304,10 +8301,10 @@
       <c r="O17" s="26"/>
       <c r="P17" s="26"/>
       <c r="Q17" s="26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R17" s="27" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="S17" s="28"/>
       <c r="T17" s="27"/>
@@ -8315,7 +8312,7 @@
       <c r="V17" s="29"/>
       <c r="W17" s="29"/>
       <c r="X17" s="29" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Y17" s="29"/>
       <c r="Z17" s="30"/>
@@ -8324,7 +8321,7 @@
     </row>
     <row r="18" spans="1:28" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="95" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B18" s="32"/>
       <c r="C18" s="25"/>
@@ -8346,10 +8343,10 @@
       <c r="O18" s="26"/>
       <c r="P18" s="26"/>
       <c r="Q18" s="26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R18" s="27" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="S18" s="28"/>
       <c r="T18" s="27"/>
@@ -8357,7 +8354,7 @@
       <c r="V18" s="29"/>
       <c r="W18" s="29"/>
       <c r="X18" s="29" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="Y18" s="29"/>
       <c r="Z18" s="30"/>
@@ -8366,7 +8363,7 @@
     </row>
     <row r="19" spans="1:28" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="95" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B19" s="32"/>
       <c r="C19" s="25"/>
@@ -8378,7 +8375,7 @@
       </c>
       <c r="H19" s="26"/>
       <c r="I19" s="26" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J19" s="26"/>
       <c r="K19" s="26"/>
@@ -8388,10 +8385,10 @@
       <c r="O19" s="26"/>
       <c r="P19" s="26"/>
       <c r="Q19" s="26" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R19" s="27" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="S19" s="28"/>
       <c r="T19" s="27"/>
@@ -8406,7 +8403,7 @@
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="95" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B20" s="25"/>
       <c r="C20" s="25"/>
@@ -8438,7 +8435,7 @@
     </row>
     <row r="21" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="95" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B21" s="32"/>
       <c r="C21" s="25"/>
@@ -8446,7 +8443,7 @@
       <c r="E21" s="25"/>
       <c r="F21" s="26"/>
       <c r="G21" s="26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H21" s="26"/>
       <c r="I21" s="26"/>
@@ -8458,31 +8455,31 @@
       <c r="O21" s="26"/>
       <c r="P21" s="26"/>
       <c r="Q21" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="R21" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="S21" s="28" t="s">
         <v>104</v>
-      </c>
-      <c r="R21" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="S21" s="28" t="s">
-        <v>106</v>
       </c>
       <c r="T21" s="27"/>
       <c r="U21" s="28"/>
       <c r="V21" s="29" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="W21" s="29"/>
       <c r="X21" s="29"/>
       <c r="Y21" s="29"/>
       <c r="Z21" s="30"/>
       <c r="AA21" s="29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AB21" s="31"/>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="95" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B22" s="32"/>
       <c r="C22" s="25"/>
@@ -8490,11 +8487,11 @@
       <c r="E22" s="25"/>
       <c r="F22" s="26"/>
       <c r="G22" s="26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H22" s="26"/>
       <c r="I22" s="26" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J22" s="26"/>
       <c r="K22" s="26"/>
@@ -8504,13 +8501,13 @@
       <c r="O22" s="26"/>
       <c r="P22" s="26"/>
       <c r="Q22" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="R22" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="S22" s="28" t="s">
         <v>110</v>
-      </c>
-      <c r="R22" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="S22" s="28" t="s">
-        <v>112</v>
       </c>
       <c r="T22" s="27"/>
       <c r="U22" s="28"/>
@@ -8524,7 +8521,7 @@
     </row>
     <row r="23" spans="1:28" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="95" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B23" s="32"/>
       <c r="C23" s="25"/>
@@ -8532,11 +8529,11 @@
       <c r="E23" s="25"/>
       <c r="F23" s="26"/>
       <c r="G23" s="26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H23" s="26"/>
       <c r="I23" s="26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J23" s="26"/>
       <c r="K23" s="26"/>
@@ -8546,13 +8543,13 @@
       <c r="O23" s="26"/>
       <c r="P23" s="26"/>
       <c r="Q23" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="R23" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="S23" s="28" t="s">
         <v>115</v>
-      </c>
-      <c r="R23" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="S23" s="28" t="s">
-        <v>117</v>
       </c>
       <c r="T23" s="27"/>
       <c r="U23" s="28"/>
@@ -8566,7 +8563,7 @@
     </row>
     <row r="24" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="95" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B24" s="32"/>
       <c r="C24" s="25"/>
@@ -8574,11 +8571,11 @@
       <c r="E24" s="25"/>
       <c r="F24" s="26"/>
       <c r="G24" s="26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H24" s="26"/>
       <c r="I24" s="26" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J24" s="26"/>
       <c r="K24" s="26"/>
@@ -8588,13 +8585,13 @@
       <c r="O24" s="26"/>
       <c r="P24" s="26"/>
       <c r="Q24" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="R24" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="S24" s="28" t="s">
         <v>120</v>
-      </c>
-      <c r="R24" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="S24" s="28" t="s">
-        <v>122</v>
       </c>
       <c r="T24" s="27"/>
       <c r="U24" s="28"/>
@@ -8608,7 +8605,7 @@
     </row>
     <row r="25" spans="1:28" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="95" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B25" s="32"/>
       <c r="C25" s="25"/>
@@ -8620,7 +8617,7 @@
       </c>
       <c r="H25" s="26"/>
       <c r="I25" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J25" s="26"/>
       <c r="K25" s="26"/>
@@ -8630,10 +8627,10 @@
       <c r="O25" s="26"/>
       <c r="P25" s="26"/>
       <c r="Q25" s="26" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="R25" s="27" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="S25" s="28"/>
       <c r="T25" s="27"/>
@@ -8648,7 +8645,7 @@
     </row>
     <row r="26" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="95" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B26" s="32"/>
       <c r="C26" s="25"/>
@@ -8656,7 +8653,7 @@
       <c r="E26" s="25"/>
       <c r="F26" s="26"/>
       <c r="G26" s="26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H26" s="26"/>
       <c r="I26" s="26" t="s">
@@ -8665,30 +8662,30 @@
       <c r="J26" s="26"/>
       <c r="K26" s="26"/>
       <c r="L26" s="26" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="M26" s="26"/>
       <c r="N26" s="26"/>
       <c r="O26" s="26"/>
       <c r="P26" s="26"/>
       <c r="Q26" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="R26" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="S26" s="28" t="s">
         <v>129</v>
-      </c>
-      <c r="R26" s="27" t="s">
-        <v>130</v>
-      </c>
-      <c r="S26" s="28" t="s">
-        <v>131</v>
       </c>
       <c r="T26" s="27"/>
       <c r="U26" s="28"/>
       <c r="V26" s="29"/>
       <c r="W26" s="29"/>
       <c r="X26" s="29" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="Y26" s="29" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="Z26" s="30"/>
       <c r="AA26" s="29"/>
@@ -8696,7 +8693,7 @@
     </row>
     <row r="27" spans="1:28" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B27" s="32"/>
       <c r="C27" s="25"/>
@@ -8708,7 +8705,7 @@
       </c>
       <c r="H27" s="26"/>
       <c r="I27" s="26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J27" s="26"/>
       <c r="K27" s="26"/>
@@ -8718,13 +8715,13 @@
       <c r="O27" s="26"/>
       <c r="P27" s="26"/>
       <c r="Q27" s="26" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R27" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="S27" s="28" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="T27" s="27"/>
       <c r="U27" s="28"/>
@@ -8738,7 +8735,7 @@
     </row>
     <row r="28" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B28" s="25"/>
       <c r="C28" s="32"/>
@@ -8750,7 +8747,7 @@
       </c>
       <c r="H28" s="26"/>
       <c r="I28" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J28" s="26"/>
       <c r="K28" s="26"/>
@@ -8760,10 +8757,10 @@
       <c r="O28" s="26"/>
       <c r="P28" s="26"/>
       <c r="Q28" s="26" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="R28" s="27" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="S28" s="28"/>
       <c r="T28" s="27"/>
@@ -8778,7 +8775,7 @@
     </row>
     <row r="29" spans="1:28" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="24" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B29" s="25"/>
       <c r="C29" s="32"/>
@@ -8790,7 +8787,7 @@
       </c>
       <c r="H29" s="26"/>
       <c r="I29" s="34" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J29" s="26"/>
       <c r="K29" s="26"/>
@@ -8800,13 +8797,13 @@
       <c r="O29" s="26"/>
       <c r="P29" s="26"/>
       <c r="Q29" s="35" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="R29" s="35" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="S29" s="28" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="T29" s="27"/>
       <c r="U29" s="28"/>
@@ -8820,7 +8817,7 @@
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="24" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B30" s="25"/>
       <c r="C30" s="32"/>
@@ -8828,11 +8825,11 @@
       <c r="E30" s="25"/>
       <c r="F30" s="26"/>
       <c r="G30" s="26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H30" s="26"/>
       <c r="I30" s="26" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J30" s="26"/>
       <c r="K30" s="26"/>
@@ -8842,10 +8839,10 @@
       <c r="O30" s="26"/>
       <c r="P30" s="26"/>
       <c r="Q30" s="35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="R30" s="35" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="T30" s="27"/>
       <c r="U30" s="28"/>
@@ -8859,7 +8856,7 @@
     </row>
     <row r="31" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B31" s="25"/>
       <c r="C31" s="25"/>
@@ -8871,7 +8868,7 @@
       </c>
       <c r="H31" s="26"/>
       <c r="I31" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J31" s="26"/>
       <c r="K31" s="26"/>
@@ -8881,10 +8878,10 @@
       <c r="O31" s="26"/>
       <c r="P31" s="26"/>
       <c r="Q31" s="26" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="R31" s="27" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="S31" s="28"/>
       <c r="T31" s="27"/>
@@ -8899,7 +8896,7 @@
     </row>
     <row r="32" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B32" s="25"/>
       <c r="C32" s="25"/>
@@ -8911,7 +8908,7 @@
       </c>
       <c r="H32" s="26"/>
       <c r="I32" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J32" s="26"/>
       <c r="K32" s="26"/>
@@ -8921,10 +8918,10 @@
       <c r="O32" s="26"/>
       <c r="P32" s="26"/>
       <c r="Q32" s="26" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="R32" s="27" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="S32" s="28"/>
       <c r="T32" s="27"/>
@@ -8939,7 +8936,7 @@
     </row>
     <row r="33" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="24" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B33" s="25"/>
       <c r="C33" s="25"/>
@@ -8951,7 +8948,7 @@
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J33" s="26"/>
       <c r="K33" s="26"/>
@@ -8961,10 +8958,10 @@
       <c r="O33" s="26"/>
       <c r="P33" s="26"/>
       <c r="Q33" s="26" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="R33" s="27" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="S33" s="28"/>
       <c r="T33" s="27"/>
@@ -11025,141 +11022,141 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34:AB101 B28:F33 A2:AB27">
-    <cfRule type="expression" dxfId="77" priority="0">
+    <cfRule type="expression" dxfId="77" priority="1">
       <formula>$G2="0..0"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="0">
+    <cfRule type="expression" dxfId="76" priority="1">
       <formula>AND(A2&lt;&gt;"",$A2="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:E11 A15:E27 A34:E101 B28:E33 A29:A33">
-    <cfRule type="expression" dxfId="75" priority="0">
+    <cfRule type="expression" dxfId="75" priority="2">
       <formula>AND(A2&lt;&gt;"",A1="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA2 G2:H2 J2:P2">
-    <cfRule type="expression" dxfId="74" priority="0">
+    <cfRule type="expression" dxfId="74" priority="3">
       <formula>G2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G101 R2:R101">
-    <cfRule type="expression" dxfId="73" priority="0">
+    <cfRule type="expression" dxfId="73" priority="4">
       <formula>($A2="")&lt;&gt;(G2="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M34:M101 P34:P101 P2:P27 M2:M27">
-    <cfRule type="expression" dxfId="72" priority="0">
+    <cfRule type="expression" dxfId="72" priority="5">
       <formula>AND(SEARCH("|",$I2)&lt;&gt;0,M2&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N34:N101 P34:P101 P2:P27 N2:N27">
-    <cfRule type="expression" dxfId="71" priority="0">
+    <cfRule type="expression" dxfId="71" priority="6">
       <formula>AND(N2&lt;&gt;"",NOT(EXACT(LEFT($I2,1),LOWER(LEFT($I2,1)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N34:O101 N2:O27">
-    <cfRule type="expression" dxfId="70" priority="0">
+    <cfRule type="expression" dxfId="70" priority="7">
       <formula>AND($N2&lt;&gt;"",$O2&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q34:R101 Q2:R27">
-    <cfRule type="expression" dxfId="69" priority="0">
+    <cfRule type="expression" dxfId="69" priority="8">
       <formula>AND($Q2&lt;&gt;"",$Q2=$R2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2:W2">
-    <cfRule type="expression" dxfId="68" priority="0">
+    <cfRule type="expression" dxfId="68" priority="9">
       <formula>V2=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3:W101">
-    <cfRule type="expression" dxfId="67" priority="0">
+    <cfRule type="expression" dxfId="67" priority="10">
       <formula>AND($A3&lt;&gt;"",ISERR(SEARCH("N/A",V$2)),V3="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2:Z10 Z34:Z101 Z12:Z27">
-    <cfRule type="expression" dxfId="66" priority="0">
+    <cfRule type="expression" dxfId="66" priority="11">
       <formula>AND(Z2&lt;&gt;"",LEFT($I2,1)&lt;&gt;"@",LEFT($A3,LEN($A2)+1)&lt;&gt;($A2&amp;"."),LEFT($A3,LEN($A2)+2)&lt;&gt;("!"&amp;$A2&amp;"."))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:AB28 A31:AB101 A29:R30 T29:AB30">
-    <cfRule type="expression" dxfId="65" priority="0">
+    <cfRule type="expression" dxfId="65" priority="12">
       <formula>LEFT($A2,1)="!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:E13">
-    <cfRule type="expression" dxfId="64" priority="0">
+    <cfRule type="expression" dxfId="64" priority="13">
       <formula>AND(A12&lt;&gt;"",A9="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:E13">
-    <cfRule type="expression" dxfId="63" priority="0">
+    <cfRule type="expression" dxfId="63" priority="14">
       <formula>AND(A13&lt;&gt;"",A11="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:E14">
-    <cfRule type="expression" dxfId="62" priority="0">
+    <cfRule type="expression" dxfId="62" priority="15">
       <formula>AND(A14&lt;&gt;"",#REF!="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z13">
-    <cfRule type="expression" dxfId="61" priority="0">
+    <cfRule type="expression" dxfId="61" priority="16">
       <formula>AND(Z13&lt;&gt;"",LEFT($I13,1)&lt;&gt;"@",LEFT(#REF!,LEN($A13)+1)&lt;&gt;($A13&amp;"."),LEFT(#REF!,LEN($A13)+2)&lt;&gt;("!"&amp;$A13&amp;"."))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z11">
-    <cfRule type="expression" dxfId="60" priority="0">
+    <cfRule type="expression" dxfId="60" priority="17">
       <formula>AND(Z11&lt;&gt;"",LEFT($I11,1)&lt;&gt;"@",LEFT(#REF!,LEN($A11)+1)&lt;&gt;($A11&amp;"."),LEFT(#REF!,LEN($A11)+2)&lt;&gt;("!"&amp;$A11&amp;"."))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:A33 G28:AB28 G31:AB33 G29:R30 T29:AB30">
-    <cfRule type="expression" dxfId="59" priority="0">
+    <cfRule type="expression" dxfId="59" priority="18">
       <formula>$C28="0..0"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="0">
+    <cfRule type="expression" dxfId="58" priority="18">
       <formula>AND(A28&lt;&gt;"",$A28="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28">
-    <cfRule type="expression" dxfId="57" priority="0">
+    <cfRule type="expression" dxfId="57" priority="19">
       <formula>AND(A28&lt;&gt;"",#REF!="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M28:M33 P28:P33">
-    <cfRule type="expression" dxfId="56" priority="0">
+    <cfRule type="expression" dxfId="56" priority="20">
       <formula>AND(SEARCH("|",$E28)&lt;&gt;0,M28&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N28:N33 P28:P33">
-    <cfRule type="expression" dxfId="55" priority="0">
+    <cfRule type="expression" dxfId="55" priority="21">
       <formula>AND(N28&lt;&gt;"",NOT(EXACT(LEFT($E28,1),LOWER(LEFT($E28,1)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N28:O33">
-    <cfRule type="expression" dxfId="54" priority="0">
+    <cfRule type="expression" dxfId="54" priority="22">
       <formula>AND($J28&lt;&gt;"",$K28&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q28:R33">
-    <cfRule type="expression" dxfId="53" priority="0">
+    <cfRule type="expression" dxfId="53" priority="23">
       <formula>AND($M28&lt;&gt;"",$M28=$N28)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z28:Z33">
-    <cfRule type="expression" dxfId="52" priority="0">
+    <cfRule type="expression" dxfId="52" priority="24">
       <formula>AND(Z28&lt;&gt;"",LEFT($E28,1)&lt;&gt;"@",LEFT($A29,LEN($A28)+1)&lt;&gt;($A28&amp;"."),LEFT($A29,LEN($A28)+2)&lt;&gt;("!"&amp;$A28&amp;"."))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S29">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="51" priority="25">
       <formula>LEFT($A30,1)="!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S29">
-    <cfRule type="expression" dxfId="1" priority="6">
+    <cfRule type="expression" dxfId="50" priority="26">
       <formula>$C30="0..0"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="7">
+    <cfRule type="expression" dxfId="49" priority="26">
       <formula>AND(S29&lt;&gt;"",$A30="")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11232,25 +11229,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="6" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="46" t="s">
         <v>155</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="D1" s="46" t="s">
         <v>156</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="E1" s="46" t="s">
         <v>157</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="F1" s="46" t="s">
         <v>158</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="G1" s="47" t="s">
         <v>159</v>
-      </c>
-      <c r="F1" s="46" t="s">
-        <v>160</v>
-      </c>
-      <c r="G1" s="47" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -11698,22 +11695,22 @@
   </sheetData>
   <autoFilter ref="A1:G2"/>
   <conditionalFormatting sqref="A2:G50">
-    <cfRule type="expression" dxfId="51" priority="0">
+    <cfRule type="expression" dxfId="48" priority="0">
       <formula>AND($A2="",A2&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A50">
-    <cfRule type="expression" dxfId="50" priority="0">
+    <cfRule type="expression" dxfId="47" priority="1">
       <formula>AND(A2&lt;&gt;"",A1="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B50 D2:E50 G2:G50">
-    <cfRule type="expression" dxfId="49" priority="0">
+    <cfRule type="expression" dxfId="46" priority="2">
       <formula>($A2&lt;&gt;"")&lt;&gt;(B2&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:G50">
-    <cfRule type="expression" dxfId="48" priority="0">
+    <cfRule type="expression" dxfId="45" priority="3">
       <formula>LEFT($A2,1)="!"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11763,49 +11760,49 @@
   <sheetData>
     <row r="1" spans="1:5" s="56" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B1" s="46" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="46" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" s="47" t="s">
         <v>162</v>
-      </c>
-      <c r="D1" s="46" t="s">
-        <v>163</v>
-      </c>
-      <c r="E1" s="47" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="57" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="58" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E2" s="59" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="60" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C3" s="26"/>
       <c r="D3" s="61" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E3" s="62" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12001,42 +11998,42 @@
   </sheetData>
   <autoFilter ref="A1:E3"/>
   <conditionalFormatting sqref="A2:E30">
-    <cfRule type="expression" dxfId="47" priority="0">
+    <cfRule type="expression" dxfId="44" priority="0">
       <formula>AND($A2="",A2&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A30">
-    <cfRule type="expression" dxfId="46" priority="0">
+    <cfRule type="expression" dxfId="43" priority="1">
       <formula>AND(A1="",A2&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B30">
-    <cfRule type="expression" dxfId="45" priority="0">
+    <cfRule type="expression" dxfId="42" priority="2">
       <formula>AND($A2&lt;&gt;"",B2="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C30">
-    <cfRule type="expression" dxfId="44" priority="0">
+    <cfRule type="expression" dxfId="41" priority="3">
       <formula>AND($A2&lt;&gt;"reference",C2&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D30">
-    <cfRule type="expression" dxfId="43" priority="0">
+    <cfRule type="expression" dxfId="40" priority="4">
       <formula>AND($B2="reference",$C2="",D2="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D30">
-    <cfRule type="expression" dxfId="42" priority="0">
+    <cfRule type="expression" dxfId="39" priority="5">
       <formula>AND($B2="reference",$C2&lt;&gt;"",D2="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E30">
-    <cfRule type="expression" dxfId="41" priority="0">
+    <cfRule type="expression" dxfId="38" priority="6">
       <formula>AND($A2&lt;&gt;"",E2="",$D2="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:E30">
-    <cfRule type="expression" dxfId="40" priority="0">
+    <cfRule type="expression" dxfId="37" priority="7">
       <formula>LEFT($A2,1)="!"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12075,31 +12072,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B1" s="68" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1" s="68" t="s">
         <v>173</v>
-      </c>
-      <c r="C1" s="68" t="s">
-        <v>174</v>
-      </c>
-      <c r="D1" s="68" t="s">
-        <v>175</v>
       </c>
       <c r="E1" s="68" t="s">
         <v>11</v>
       </c>
       <c r="F1" s="68" t="s">
+        <v>174</v>
+      </c>
+      <c r="G1" s="68" t="s">
+        <v>175</v>
+      </c>
+      <c r="H1" s="69" t="s">
         <v>176</v>
       </c>
-      <c r="G1" s="68" t="s">
+      <c r="I1" s="70" t="s">
         <v>177</v>
-      </c>
-      <c r="H1" s="69" t="s">
-        <v>178</v>
-      </c>
-      <c r="I1" s="70" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12645,60 +12642,60 @@
   </sheetData>
   <autoFilter ref="A1:I2"/>
   <conditionalFormatting sqref="A2:I50">
-    <cfRule type="expression" dxfId="39" priority="0">
+    <cfRule type="expression" dxfId="36" priority="0">
       <formula>AND($A2="",A2&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A50">
-    <cfRule type="expression" dxfId="38" priority="0">
+    <cfRule type="expression" dxfId="35" priority="1">
       <formula>AND(A1="",A2&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B50 E2:E50 H2:H50">
-    <cfRule type="expression" dxfId="37" priority="0">
+    <cfRule type="expression" dxfId="34" priority="2">
       <formula>AND($A2&lt;&gt;"",B2="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B50">
-    <cfRule type="expression" dxfId="36" priority="0">
+    <cfRule type="expression" dxfId="33" priority="3">
       <formula>AND($A2&lt;&gt;"",NOT(ISERR(SEARCH(".",$A2))),B2&lt;&gt;"IN", B2&lt;&gt;"OUT")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C50">
-    <cfRule type="expression" dxfId="35" priority="0">
+    <cfRule type="expression" dxfId="32" priority="4">
       <formula>AND(C2&lt;&gt;"",ISERR(VALUE(C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:D50">
-    <cfRule type="expression" dxfId="34" priority="0">
+    <cfRule type="expression" dxfId="31" priority="5">
       <formula>AND($A2&lt;&gt;"",ISERR(SEARCH(".",$A2))&lt;&gt;(C2=""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D50">
-    <cfRule type="expression" dxfId="33" priority="0">
+    <cfRule type="expression" dxfId="30" priority="6">
       <formula>AND($C2&lt;&gt;"",D2&lt;&gt;"",D2&lt;&gt;"*",D2&lt;$C2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="0">
+    <cfRule type="expression" dxfId="29" priority="6">
       <formula>AND(D2&lt;&gt;"",D2&lt;&gt;"*",ISERR(VALUE(D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E50">
-    <cfRule type="expression" priority="0">
+    <cfRule type="expression" priority="7">
       <formula>AND($A2&lt;&gt;"",NOT(ISERR(SEARCH(".",$A2))),$B2&lt;&gt;"QUERY", $B2&lt;&gt;"OPERATION")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F50">
-    <cfRule type="expression" dxfId="31" priority="0">
+    <cfRule type="expression" dxfId="28" priority="8">
       <formula>AND($A2&lt;&gt;"",ISERR(SEARCH(".",$A2)),(F2&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I50">
-    <cfRule type="expression" dxfId="30" priority="0">
+    <cfRule type="expression" dxfId="27" priority="9">
       <formula>AND($A2&lt;&gt;"",NOT(ISERR(SEARCH(".",$A2))),I2&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:I50">
-    <cfRule type="expression" dxfId="29" priority="0">
+    <cfRule type="expression" dxfId="26" priority="10">
       <formula>LEFT($A2,1)="!"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12744,31 +12741,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>162</v>
+      </c>
+      <c r="D1" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="E1" s="46" t="s">
         <v>181</v>
       </c>
-      <c r="C1" s="46" t="s">
-        <v>164</v>
-      </c>
-      <c r="D1" s="46" t="s">
+      <c r="F1" s="46" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="G1" s="46" t="s">
         <v>183</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="H1" s="46" t="s">
         <v>184</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="I1" s="47" t="s">
         <v>185</v>
-      </c>
-      <c r="H1" s="46" t="s">
-        <v>186</v>
-      </c>
-      <c r="I1" s="47" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12984,22 +12981,22 @@
   </sheetData>
   <autoFilter ref="A1:I1"/>
   <conditionalFormatting sqref="A2:I20">
-    <cfRule type="expression" dxfId="28" priority="0">
+    <cfRule type="expression" dxfId="25" priority="0">
       <formula>AND($A2="",A2&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A20">
-    <cfRule type="expression" dxfId="27" priority="0">
+    <cfRule type="expression" dxfId="24" priority="1">
       <formula>AND(A2&lt;&gt;"",A1="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C20">
-    <cfRule type="expression" dxfId="26" priority="0">
+    <cfRule type="expression" dxfId="23" priority="2">
       <formula>($A2&lt;&gt;"")&lt;&gt;(B2&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:I20">
-    <cfRule type="expression" dxfId="25" priority="0">
+    <cfRule type="expression" dxfId="22" priority="3">
       <formula>LEFT($A2,1)="!"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13036,13 +13033,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B1" s="46" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C1" s="46" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D1" s="47" t="s">
         <v>11</v>
@@ -13286,22 +13283,22 @@
   </sheetData>
   <autoFilter ref="A1:D2"/>
   <conditionalFormatting sqref="A2:D40">
-    <cfRule type="expression" dxfId="24" priority="0">
+    <cfRule type="expression" dxfId="21" priority="0">
       <formula>AND($A2="",A2&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A40">
-    <cfRule type="expression" dxfId="23" priority="0">
+    <cfRule type="expression" dxfId="20" priority="1">
       <formula>AND(A2&lt;&gt;"",A1="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B40 D2:D40">
-    <cfRule type="expression" dxfId="22" priority="0">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>AND($A2&lt;&gt;"",B2="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:D40">
-    <cfRule type="expression" dxfId="21" priority="0">
+    <cfRule type="expression" dxfId="18" priority="3">
       <formula>LEFT($A2,1)="!"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13339,44 +13336,44 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B1" s="46" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="80" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E1" s="46" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F1" s="46" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G1" s="47" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="81" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D2" s="16">
         <v>87654</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F2" s="71"/>
       <c r="G2" s="82" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -13725,27 +13722,27 @@
   </sheetData>
   <autoFilter ref="A1:G2"/>
   <conditionalFormatting sqref="A2:G40">
-    <cfRule type="expression" dxfId="20" priority="0">
+    <cfRule type="expression" dxfId="17" priority="0">
       <formula>AND($A2="",A2&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A40">
-    <cfRule type="expression" dxfId="19" priority="0">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>AND(A2&lt;&gt;"",A1="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C40 E2:E40">
-    <cfRule type="expression" dxfId="18" priority="0">
+    <cfRule type="expression" dxfId="15" priority="2">
       <formula>AND($A2&lt;&gt;"",C2="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:G40">
-    <cfRule type="expression" dxfId="17" priority="0">
+    <cfRule type="expression" dxfId="14" priority="3">
       <formula>LEFT($A2,1)="!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D40">
-    <cfRule type="expression" dxfId="16" priority="0">
+    <cfRule type="expression" dxfId="13" priority="4">
       <formula>AND($A2&lt;&gt;"",OR($B2="",$B2="xml"),D2="")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13793,7 +13790,7 @@
         <v>10</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>28</v>
@@ -13805,7 +13802,7 @@
         <v>14</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>20</v>
@@ -13817,7 +13814,7 @@
         <v>22</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="M1" s="6" t="s">
         <v>24</v>
@@ -13833,7 +13830,7 @@
       </c>
       <c r="Q1" s="6"/>
       <c r="R1" s="6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="T1" s="88" t="s">
         <v>15</v>

</xml_diff>